<commit_message>
Historical Data + Observation balanced
</commit_message>
<xml_diff>
--- a/Phase7_Python/output.xlsx
+++ b/Phase7_Python/output.xlsx
@@ -539,7 +539,7 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>-0.08599999999999999</v>
+        <v>-0.043</v>
       </c>
       <c r="B14" t="n">
         <v>0</v>
@@ -547,7 +547,7 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.02500974846757485</v>
       </c>
       <c r="B15" t="n">
         <v>0</v>
@@ -555,7 +555,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>0</v>
+        <v>0.01011255226241359</v>
       </c>
       <c r="B16" t="n">
         <v>0</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>0</v>
+        <v>0.004119126160510491</v>
       </c>
       <c r="B17" t="n">
         <v>0</v>
@@ -571,7 +571,7 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>0</v>
+        <v>0.001705323875853631</v>
       </c>
       <c r="B18" t="n">
         <v>0</v>
@@ -579,7 +579,7 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>0</v>
+        <v>0.0007308661625607839</v>
       </c>
       <c r="B19" t="n">
         <v>0</v>
@@ -587,7 +587,7 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>0</v>
+        <v>0.0003353541268450571</v>
       </c>
       <c r="B20" t="n">
         <v>0</v>
@@ -595,7 +595,7 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>0</v>
+        <v>0.0001728885105065577</v>
       </c>
       <c r="B21" t="n">
         <v>0</v>
@@ -603,7 +603,7 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>0</v>
+        <v>0.0001043953354888498</v>
       </c>
       <c r="B22" t="n">
         <v>0</v>
@@ -611,7 +611,7 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
-        <v>0</v>
+        <v>7.394419381824675e-05</v>
       </c>
       <c r="B23" t="n">
         <v>0</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>0</v>
+        <v>-0.001300719012366395</v>
       </c>
       <c r="B24" t="n">
         <v>0</v>
@@ -627,7 +627,7 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>0</v>
+        <v>0.0004085295033821824</v>
       </c>
       <c r="B25" t="n">
         <v>0</v>
@@ -635,7 +635,7 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>0</v>
+        <v>0.0005466724865793977</v>
       </c>
       <c r="B26" t="n">
         <v>0</v>
@@ -643,7 +643,7 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>0</v>
+        <v>0.0003807032260573495</v>
       </c>
       <c r="B27" t="n">
         <v>0</v>
@@ -651,7 +651,7 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>0</v>
+        <v>0.000224199255663536</v>
       </c>
       <c r="B28" t="n">
         <v>0</v>
@@ -659,7 +659,7 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.04312452232452622</v>
       </c>
       <c r="B29" t="n">
         <v>0</v>
@@ -667,7 +667,7 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>0</v>
+        <v>0.01805932205361653</v>
       </c>
       <c r="B30" t="n">
         <v>0</v>
@@ -675,7 +675,7 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.0509177515468736</v>
       </c>
       <c r="B31" t="n">
         <v>0</v>
@@ -683,7 +683,7 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.0647740187286899</v>
       </c>
       <c r="B32" t="n">
         <v>0</v>
@@ -691,7 +691,7 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>0</v>
+        <v>0.02793869806126089</v>
       </c>
       <c r="B33" t="n">
         <v>0</v>
@@ -699,7 +699,7 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>0</v>
+        <v>0.01292897383639191</v>
       </c>
       <c r="B34" t="n">
         <v>0</v>
@@ -707,7 +707,7 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>0</v>
+        <v>0.006807323770054493</v>
       </c>
       <c r="B35" t="n">
         <v>0</v>
@@ -715,7 +715,7 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>0</v>
+        <v>0.004216245090050301</v>
       </c>
       <c r="B36" t="n">
         <v>0</v>
@@ -723,7 +723,7 @@
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>0</v>
+        <v>0.003045688312774996</v>
       </c>
       <c r="B37" t="n">
         <v>0</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>0</v>
+        <v>0.002457247622277219</v>
       </c>
       <c r="B38" t="n">
         <v>0</v>
@@ -739,7 +739,7 @@
     </row>
     <row r="39">
       <c r="A39" t="n">
-        <v>0</v>
+        <v>0.003474213148185527</v>
       </c>
       <c r="B39" t="n">
         <v>0</v>
@@ -747,7 +747,7 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>0</v>
+        <v>0.002882516957575471</v>
       </c>
       <c r="B40" t="n">
         <v>0</v>
@@ -755,7 +755,7 @@
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>0</v>
+        <v>0.003559474427378824</v>
       </c>
       <c r="B41" t="n">
         <v>0</v>
@@ -763,7 +763,7 @@
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>0</v>
+        <v>0.004069040581945269</v>
       </c>
       <c r="B42" t="n">
         <v>0</v>
@@ -771,7 +771,7 @@
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>0</v>
+        <v>0.002888492860535875</v>
       </c>
       <c r="B43" t="n">
         <v>0</v>
@@ -779,7 +779,7 @@
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>0</v>
+        <v>0.001834542115959247</v>
       </c>
       <c r="B44" t="n">
         <v>0</v>
@@ -787,7 +787,7 @@
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>0</v>
+        <v>0.001160983633565649</v>
       </c>
       <c r="B45" t="n">
         <v>0</v>
@@ -795,7 +795,7 @@
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>0</v>
+        <v>0.0007728751252033038</v>
       </c>
       <c r="B46" t="n">
         <v>0</v>
@@ -803,7 +803,7 @@
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>0</v>
+        <v>0.0005542453415374798</v>
       </c>
       <c r="B47" t="n">
         <v>0</v>
@@ -811,7 +811,7 @@
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>0</v>
+        <v>0.0004273869792766666</v>
       </c>
       <c r="B48" t="n">
         <v>0</v>
@@ -819,7 +819,7 @@
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>0</v>
+        <v>0.0003914443500390536</v>
       </c>
       <c r="B49" t="n">
         <v>0</v>
@@ -827,7 +827,7 @@
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.04333992100983215</v>
       </c>
       <c r="B50" t="n">
         <v>0</v>
@@ -835,7 +835,7 @@
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>0</v>
+        <v>0.01831560321766129</v>
       </c>
       <c r="B51" t="n">
         <v>0</v>
@@ -843,7 +843,7 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>0</v>
+        <v>0.008197529883347331</v>
       </c>
       <c r="B52" t="n">
         <v>0</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>0</v>
+        <v>0.004023047003269681</v>
       </c>
       <c r="B53" t="n">
         <v>0</v>
@@ -859,7 +859,7 @@
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>0</v>
+        <v>0.002250779147337127</v>
       </c>
       <c r="B54" t="n">
         <v>0</v>
@@ -867,7 +867,7 @@
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>0</v>
+        <v>0.001464076498457242</v>
       </c>
       <c r="B55" t="n">
         <v>0</v>
@@ -875,7 +875,7 @@
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>0</v>
+        <v>0.001088795980767381</v>
       </c>
       <c r="B56" t="n">
         <v>0</v>
@@ -883,7 +883,7 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>0</v>
+        <v>0.0008891975931538497</v>
       </c>
       <c r="B57" t="n">
         <v>0</v>
@@ -891,7 +891,7 @@
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>0</v>
+        <v>0.0007671985477066683</v>
       </c>
       <c r="B58" t="n">
         <v>0</v>
@@ -899,7 +899,7 @@
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>0</v>
+        <v>0.0006827602830742287</v>
       </c>
       <c r="B59" t="n">
         <v>0</v>
@@ -907,7 +907,7 @@
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>0</v>
+        <v>0.001975636268271412</v>
       </c>
       <c r="B60" t="n">
         <v>0</v>
@@ -915,7 +915,7 @@
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>0</v>
+        <v>0.00156180103708447</v>
       </c>
       <c r="B61" t="n">
         <v>0</v>
@@ -923,7 +923,7 @@
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>0</v>
+        <v>0.001011308918576205</v>
       </c>
       <c r="B62" t="n">
         <v>0</v>
@@ -931,7 +931,7 @@
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>0</v>
+        <v>0.0006259485814173581</v>
       </c>
       <c r="B63" t="n">
         <v>0</v>
@@ -939,7 +939,7 @@
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>0</v>
+        <v>0.0003966501483359614</v>
       </c>
       <c r="B64" t="n">
         <v>0</v>
@@ -947,7 +947,7 @@
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>0</v>
+        <v>0.0002674719995877265</v>
       </c>
       <c r="B65" t="n">
         <v>0</v>
@@ -955,7 +955,7 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>0</v>
+        <v>0.0001946448768756761</v>
       </c>
       <c r="B66" t="n">
         <v>0</v>
@@ -963,7 +963,7 @@
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>0</v>
+        <v>0.00015177301573353</v>
       </c>
       <c r="B67" t="n">
         <v>0</v>
@@ -971,7 +971,7 @@
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>0</v>
+        <v>0.0001245334561271512</v>
       </c>
       <c r="B68" t="n">
         <v>0</v>
@@ -979,7 +979,7 @@
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>0</v>
+        <v>0.0001056022187455339</v>
       </c>
       <c r="B69" t="n">
         <v>0</v>
@@ -987,7 +987,7 @@
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>0</v>
+        <v>0.0001342316561266602</v>
       </c>
       <c r="B70" t="n">
         <v>0</v>
@@ -995,7 +995,7 @@
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>0</v>
+        <v>0.000124980205132279</v>
       </c>
       <c r="B71" t="n">
         <v>0</v>
@@ -1003,7 +1003,7 @@
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>0</v>
+        <v>9.791547103044294e-05</v>
       </c>
       <c r="B72" t="n">
         <v>0</v>
@@ -1011,7 +1011,7 @@
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>0</v>
+        <v>7.086375971735903e-05</v>
       </c>
       <c r="B73" t="n">
         <v>0</v>
@@ -1019,7 +1019,7 @@
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>0</v>
+        <v>5.010442976447844e-05</v>
       </c>
       <c r="B74" t="n">
         <v>0</v>
@@ -1027,7 +1027,7 @@
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>0</v>
+        <v>3.586705018549163e-05</v>
       </c>
       <c r="B75" t="n">
         <v>0</v>
@@ -1035,7 +1035,7 @@
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>0</v>
+        <v>2.652601762506913e-05</v>
       </c>
       <c r="B76" t="n">
         <v>0</v>
@@ -1043,7 +1043,7 @@
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>0</v>
+        <v>2.040298993405333e-05</v>
       </c>
       <c r="B77" t="n">
         <v>0</v>
@@ -1051,7 +1051,7 @@
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>0</v>
+        <v>1.626588117693481e-05</v>
       </c>
       <c r="B78" t="n">
         <v>0</v>
@@ -1059,7 +1059,7 @@
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>0</v>
+        <v>1.332992283090886e-05</v>
       </c>
       <c r="B79" t="n">
         <v>0</v>
@@ -1067,7 +1067,7 @@
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.04301248720610602</v>
       </c>
       <c r="B80" t="n">
         <v>0</v>
@@ -1075,7 +1075,7 @@
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>0</v>
+        <v>0.01800151139005832</v>
       </c>
       <c r="B81" t="n">
         <v>0</v>
@@ -1083,7 +1083,7 @@
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.05088708816408288</v>
       </c>
       <c r="B82" t="n">
         <v>0</v>
@@ -1091,7 +1091,7 @@
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>0</v>
+        <v>0.02175619943881884</v>
       </c>
       <c r="B83" t="n">
         <v>0</v>
@@ -1099,7 +1099,7 @@
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.05293655615900901</v>
       </c>
       <c r="B84" t="n">
         <v>0</v>
@@ -1107,7 +1107,7 @@
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>0</v>
+        <v>0.02307543379439556</v>
       </c>
       <c r="B85" t="n">
         <v>0</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>0</v>
+        <v>0.01092118790117083</v>
       </c>
       <c r="B86" t="n">
         <v>0</v>
@@ -1123,7 +1123,7 @@
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>0</v>
+        <v>0.00589757878720194</v>
       </c>
       <c r="B87" t="n">
         <v>0</v>
@@ -1131,7 +1131,7 @@
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>0</v>
+        <v>0.003751982234047814</v>
       </c>
       <c r="B88" t="n">
         <v>0</v>
@@ -1139,7 +1139,7 @@
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>0</v>
+        <v>0.002773899837370361</v>
       </c>
       <c r="B89" t="n">
         <v>0</v>
@@ -1147,7 +1147,7 @@
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>0</v>
+        <v>0.003634622683644521</v>
       </c>
       <c r="B90" t="n">
         <v>0</v>
@@ -1155,7 +1155,7 @@
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>0</v>
+        <v>0.002979064348212647</v>
       </c>
       <c r="B91" t="n">
         <v>0</v>
@@ -1163,7 +1163,7 @@
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>0</v>
+        <v>0.003628527495834017</v>
       </c>
       <c r="B92" t="n">
         <v>0</v>
@@ -1171,7 +1171,7 @@
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>0</v>
+        <v>0.002765170384207243</v>
       </c>
       <c r="B93" t="n">
         <v>0</v>
@@ -1179,7 +1179,7 @@
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>0</v>
+        <v>0.003294857177979196</v>
       </c>
       <c r="B94" t="n">
         <v>0</v>
@@ -1187,7 +1187,7 @@
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>0</v>
+        <v>0.002380969125391943</v>
       </c>
       <c r="B95" t="n">
         <v>0</v>
@@ -1195,7 +1195,7 @@
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>0</v>
+        <v>0.001540922207417683</v>
       </c>
       <c r="B96" t="n">
         <v>0</v>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>0</v>
+        <v>0.0009955644860197045</v>
       </c>
       <c r="B97" t="n">
         <v>0</v>
@@ -1211,7 +1211,7 @@
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>0.172</v>
+        <v>0.08667704032899129</v>
       </c>
       <c r="B98" t="n">
         <v>0</v>
@@ -1219,7 +1219,7 @@
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>0</v>
+        <v>0.03647542512607743</v>
       </c>
       <c r="B99" t="n">
         <v>0</v>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>0</v>
+        <v>0.01618570397263527</v>
       </c>
       <c r="B100" t="n">
         <v>0</v>
@@ -1235,7 +1235,7 @@
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>0</v>
+        <v>0.007881402935973267</v>
       </c>
       <c r="B101" t="n">
         <v>0</v>
@@ -1243,7 +1243,7 @@
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>0</v>
+        <v>0.0044487488193611</v>
       </c>
       <c r="B102" t="n">
         <v>0</v>
@@ -1251,7 +1251,7 @@
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>0</v>
+        <v>0.00293449618908012</v>
       </c>
       <c r="B103" t="n">
         <v>0</v>
@@ -1259,7 +1259,7 @@
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>0</v>
+        <v>0.002246703897273532</v>
       </c>
       <c r="B104" t="n">
         <v>0</v>
@@ -1267,7 +1267,7 @@
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>0</v>
+        <v>0.001852102172565204</v>
       </c>
       <c r="B105" t="n">
         <v>0</v>
@@ -1275,7 +1275,7 @@
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>0</v>
+        <v>0.001587570480590079</v>
       </c>
       <c r="B106" t="n">
         <v>0</v>
@@ -1283,7 +1283,7 @@
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>0</v>
+        <v>0.001393498982952785</v>
       </c>
       <c r="B107" t="n">
         <v>0</v>
@@ -1291,7 +1291,7 @@
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>0</v>
+        <v>0.003961756920762885</v>
       </c>
       <c r="B108" t="n">
         <v>0</v>
@@ -1299,7 +1299,7 @@
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>0</v>
+        <v>0.003122280293169279</v>
       </c>
       <c r="B109" t="n">
         <v>0</v>
@@ -1307,7 +1307,7 @@
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>0</v>
+        <v>0.00201531887891573</v>
       </c>
       <c r="B110" t="n">
         <v>0</v>
@@ -1315,7 +1315,7 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>0</v>
+        <v>0.001244173682706068</v>
       </c>
       <c r="B111" t="n">
         <v>0</v>
@@ -1323,7 +1323,7 @@
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>0</v>
+        <v>0.0007893445322740134</v>
       </c>
       <c r="B112" t="n">
         <v>0</v>
@@ -1331,7 +1331,7 @@
     </row>
     <row r="113">
       <c r="A113" t="n">
-        <v>0</v>
+        <v>0.0005344444954122028</v>
       </c>
       <c r="B113" t="n">
         <v>0</v>
@@ -1339,7 +1339,7 @@
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>0</v>
+        <v>0.0003920733121692828</v>
       </c>
       <c r="B114" t="n">
         <v>0</v>
@@ -1347,7 +1347,7 @@
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>0</v>
+        <v>0.0003075451246070654</v>
       </c>
       <c r="B115" t="n">
         <v>0</v>
@@ -1355,7 +1355,7 @@
     </row>
     <row r="116">
       <c r="A116" t="n">
-        <v>0</v>
+        <v>0.0005355573469910585</v>
       </c>
       <c r="B116" t="n">
         <v>0</v>
@@ -1363,7 +1363,7 @@
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>0</v>
+        <v>0.0003320336616722943</v>
       </c>
       <c r="B117" t="n">
         <v>0</v>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>0</v>
+        <v>0.0003216719420077228</v>
       </c>
       <c r="B118" t="n">
         <v>0</v>
@@ -1379,7 +1379,7 @@
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>0</v>
+        <v>0.0002752253378438344</v>
       </c>
       <c r="B119" t="n">
         <v>0</v>
@@ -1387,7 +1387,7 @@
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>0</v>
+        <v>0.0002093497691033002</v>
       </c>
       <c r="B120" t="n">
         <v>0</v>
@@ -1395,650 +1395,650 @@
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.04315022997651986</v>
       </c>
       <c r="B121" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.043</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>0</v>
+        <v>0.0180968089490638</v>
       </c>
       <c r="B122" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.06099025153242515</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>-0.08599999999999999</v>
+        <v>-0.03504521965553267</v>
       </c>
       <c r="B123" t="n">
-        <v>0</v>
+        <v>0.02586795080243671</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>0</v>
+        <v>-0.01417381190620678</v>
       </c>
       <c r="B124" t="n">
-        <v>0</v>
+        <v>0.01163627237951264</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>0</v>
+        <v>-0.005779228019928414</v>
       </c>
       <c r="B125" t="n">
-        <v>0</v>
+        <v>0.00581182234314852</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>0</v>
+        <v>-0.002390676862218801</v>
       </c>
       <c r="B126" t="n">
-        <v>0</v>
+        <v>0.003375632304734106</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>0</v>
+        <v>-0.001029311352843132</v>
       </c>
       <c r="B127" t="n">
-        <v>0</v>
+        <v>0.002309412015328266</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>0</v>
+        <v>-0.0004766764186046178</v>
       </c>
       <c r="B128" t="n">
-        <v>0</v>
+        <v>0.001801169377976651</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>0</v>
+        <v>-0.0002507328147649129</v>
       </c>
       <c r="B129" t="n">
-        <v>0</v>
+        <v>0.001523885531981243</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>0</v>
+        <v>-0.0001570466551122954</v>
       </c>
       <c r="B130" t="n">
-        <v>0</v>
+        <v>0.001345546002674146</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>0</v>
+        <v>0.001243196570488766</v>
       </c>
       <c r="B131" t="n">
-        <v>0</v>
+        <v>0.002572320821222294</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>0</v>
+        <v>0.000904614743138846</v>
       </c>
       <c r="B132" t="n">
-        <v>0</v>
+        <v>0.003464510330206506</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>0</v>
+        <v>-0.0009458023490983216</v>
       </c>
       <c r="B133" t="n">
-        <v>0</v>
+        <v>0.002509308340244927</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
-        <v>0</v>
+        <v>-0.0009201682194959589</v>
       </c>
       <c r="B134" t="n">
-        <v>0</v>
+        <v>0.00158193262760818</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>0</v>
+        <v>-0.0005992627472185626</v>
       </c>
       <c r="B135" t="n">
-        <v>0</v>
+        <v>0.0009770301458872947</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="n">
-        <v>0</v>
+        <v>-0.0003439321530436747</v>
       </c>
       <c r="B136" t="n">
-        <v>0</v>
+        <v>0.0006283085656975313</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.04281037179183727</v>
       </c>
       <c r="B137" t="n">
-        <v>0</v>
+        <v>0.000434715719979924</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>0</v>
+        <v>0.01788442235802681</v>
       </c>
       <c r="B138" t="n">
-        <v>0</v>
+        <v>0.0003255929219265107</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
-        <v>0</v>
+        <v>0.007815176071590846</v>
       </c>
       <c r="B139" t="n">
-        <v>0</v>
+        <v>0.0002603465583007988</v>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="n">
-        <v>0</v>
+        <v>0.003718091586451702</v>
       </c>
       <c r="B140" t="n">
-        <v>0</v>
+        <v>0.0002176544463603938</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="n">
-        <v>0</v>
+        <v>0.002067190025409175</v>
       </c>
       <c r="B141" t="n">
-        <v>0</v>
+        <v>0.0002298380353910669</v>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="n">
-        <v>-0.08599999999999999</v>
+        <v>-0.04165503185035138</v>
       </c>
       <c r="B142" t="n">
-        <v>0</v>
+        <v>0.0002510471669340996</v>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
-        <v>0</v>
+        <v>-0.01703709639444062</v>
       </c>
       <c r="B143" t="n">
-        <v>0</v>
+        <v>0.0002161023326885859</v>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
-        <v>0</v>
+        <v>-0.007115726556135378</v>
       </c>
       <c r="B144" t="n">
-        <v>0</v>
+        <v>0.0001630987819069057</v>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="n">
-        <v>0</v>
+        <v>-0.003094978728116122</v>
       </c>
       <c r="B145" t="n">
-        <v>0</v>
+        <v>0.0001162902428337539</v>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="n">
-        <v>0</v>
+        <v>-0.001451000900351446</v>
       </c>
       <c r="B146" t="n">
-        <v>0</v>
+        <v>8.220520355119669e-05</v>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="n">
-        <v>0</v>
+        <v>0.0005917821903366723</v>
       </c>
       <c r="B147" t="n">
-        <v>0</v>
+        <v>5.941696265209575e-05</v>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="n">
-        <v>0</v>
+        <v>0.0005264995095922274</v>
       </c>
       <c r="B148" t="n">
-        <v>0</v>
+        <v>4.46007418391685e-05</v>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="n">
-        <v>0</v>
+        <v>0.0001577155505935914</v>
       </c>
       <c r="B149" t="n">
-        <v>0</v>
+        <v>3.484951155205628e-05</v>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="n">
-        <v>0</v>
+        <v>-0.0001155803437234041</v>
       </c>
       <c r="B150" t="n">
-        <v>0</v>
+        <v>2.816488540964045e-05</v>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="n">
-        <v>0</v>
+        <v>-0.000262682409711764</v>
       </c>
       <c r="B151" t="n">
-        <v>0</v>
+        <v>2.467944246515676e-05</v>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="n">
-        <v>0</v>
+        <v>-0.001686324054824501</v>
       </c>
       <c r="B152" t="n">
-        <v>0</v>
+        <v>2.283218641565924e-05</v>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="n">
-        <v>0</v>
+        <v>-0.001347976264631882</v>
       </c>
       <c r="B153" t="n">
-        <v>0</v>
+        <v>1.990506115804304e-05</v>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
-        <v>0</v>
+        <v>-0.0008422034621916799</v>
       </c>
       <c r="B154" t="n">
-        <v>0</v>
+        <v>1.615543839551367e-05</v>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="n">
-        <v>0</v>
+        <v>-0.0004866334261386898</v>
       </c>
       <c r="B155" t="n">
-        <v>0</v>
+        <v>1.248620584819594e-05</v>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
-        <v>0</v>
+        <v>-0.0002793316352851764</v>
       </c>
       <c r="B156" t="n">
-        <v>0</v>
+        <v>9.432392150852203e-06</v>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
-        <v>1.29</v>
+        <v>0.6448755973578137</v>
       </c>
       <c r="B157" t="n">
-        <v>1.204</v>
+        <v>0.602007115203875</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="n">
-        <v>1.118</v>
+        <v>0.8287905985273527</v>
       </c>
       <c r="B158" t="n">
-        <v>1.204</v>
+        <v>0.8538689587771988</v>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
-        <v>0.8599999999999999</v>
+        <v>0.7819896366402559</v>
       </c>
       <c r="B159" t="n">
-        <v>1.204</v>
+        <v>0.9641555502430208</v>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="n">
-        <v>0.7739999999999999</v>
+        <v>0.7256410705774397</v>
       </c>
       <c r="B160" t="n">
-        <v>1.204</v>
+        <v>1.016774709011388</v>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="n">
-        <v>0.516</v>
+        <v>0.5782967965430958</v>
       </c>
       <c r="B161" t="n">
-        <v>1.204</v>
+        <v>1.045519600793141</v>
       </c>
     </row>
     <row r="162">
       <c r="A162" t="n">
-        <v>0.344</v>
+        <v>0.4348585577133387</v>
       </c>
       <c r="B162" t="n">
-        <v>1.118</v>
+        <v>1.021032546434686</v>
       </c>
     </row>
     <row r="163">
       <c r="A163" t="n">
-        <v>0.172</v>
+        <v>0.2914868457685507</v>
       </c>
       <c r="B163" t="n">
-        <v>1.204</v>
+        <v>1.059860335845972</v>
       </c>
     </row>
     <row r="164">
       <c r="A164" t="n">
-        <v>0.08599999999999999</v>
+        <v>0.1897135207813607</v>
       </c>
       <c r="B164" t="n">
-        <v>1.204</v>
+        <v>1.081370501662486</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
-        <v>-0.08599999999999999</v>
+        <v>0.06104804052655546</v>
       </c>
       <c r="B165" t="n">
-        <v>1.204</v>
+        <v>1.095425731179465</v>
       </c>
     </row>
     <row r="166">
       <c r="A166" t="n">
-        <v>-0.344</v>
+        <v>-0.1226953310924225</v>
       </c>
       <c r="B166" t="n">
-        <v>1.204</v>
+        <v>1.10603198458506</v>
       </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
-        <v>0</v>
+        <v>-0.009046443556725889</v>
       </c>
       <c r="B167" t="n">
-        <v>0</v>
+        <v>0.5318739004359955</v>
       </c>
     </row>
     <row r="168">
       <c r="A168" t="n">
-        <v>0</v>
+        <v>0.03908739271297178</v>
       </c>
       <c r="B168" t="n">
-        <v>0</v>
+        <v>0.3017374213105422</v>
       </c>
     </row>
     <row r="169">
       <c r="A169" t="n">
-        <v>0.09674999999999999</v>
+        <v>0.08783901744759995</v>
       </c>
       <c r="B169" t="n">
-        <v>0.1505</v>
+        <v>0.4508529431687903</v>
       </c>
     </row>
     <row r="170">
       <c r="A170" t="n">
-        <v>-1.978</v>
+        <v>-0.9203848119433787</v>
       </c>
       <c r="B170" t="n">
-        <v>2.408</v>
+        <v>1.467962195192188</v>
       </c>
     </row>
     <row r="171">
       <c r="A171" t="n">
-        <v>-2.322</v>
+        <v>-1.521332320401143</v>
       </c>
       <c r="B171" t="n">
-        <v>2.408</v>
+        <v>1.890553671724631</v>
       </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
-        <v>-2.666</v>
+        <v>-1.959277323385634</v>
       </c>
       <c r="B172" t="n">
-        <v>2.322</v>
+        <v>2.028325035791736</v>
       </c>
     </row>
     <row r="173">
       <c r="A173" t="n">
-        <v>-3.01</v>
+        <v>-2.332476444896667</v>
       </c>
       <c r="B173" t="n">
-        <v>2.408</v>
+        <v>2.137988530233303</v>
       </c>
     </row>
     <row r="174">
       <c r="A174" t="n">
-        <v>-3.354</v>
+        <v>-2.679049229142675</v>
       </c>
       <c r="B174" t="n">
-        <v>2.408</v>
+        <v>2.192566911881764</v>
       </c>
     </row>
     <row r="175">
       <c r="A175" t="n">
-        <v>-3.698</v>
+        <v>-3.016535204112424</v>
       </c>
       <c r="B175" t="n">
-        <v>2.408</v>
+        <v>2.223888493504918</v>
       </c>
     </row>
     <row r="176">
       <c r="A176" t="n">
-        <v>-3.956</v>
+        <v>-3.309741176468953</v>
       </c>
       <c r="B176" t="n">
-        <v>2.408</v>
+        <v>2.24496764018128</v>
       </c>
     </row>
     <row r="177">
       <c r="A177" t="n">
-        <v>-4.3</v>
+        <v>-3.618470918861052</v>
       </c>
       <c r="B177" t="n">
-        <v>2.322</v>
+        <v>2.199728290971636</v>
       </c>
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>-4.643999999999999</v>
+        <v>-3.936754509311614</v>
       </c>
       <c r="B178" t="n">
-        <v>2.408</v>
+        <v>2.224899309086591</v>
       </c>
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>-4.901999999999999</v>
+        <v>-4.216823811389187</v>
       </c>
       <c r="B179" t="n">
-        <v>2.322</v>
+        <v>2.205042131088227</v>
       </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>-5.246</v>
+        <v>-4.558136085898945</v>
       </c>
       <c r="B180" t="n">
-        <v>2.322</v>
+        <v>2.235738165291415</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>-5.59</v>
+        <v>-4.909264391675093</v>
       </c>
       <c r="B181" t="n">
-        <v>2.408</v>
+        <v>2.307722210874556</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>-5.933999999999999</v>
+        <v>-5.258497816982935</v>
       </c>
       <c r="B182" t="n">
-        <v>2.322</v>
+        <v>2.30061004892442</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>-6.106</v>
+        <v>-5.518724140877545</v>
       </c>
       <c r="B183" t="n">
-        <v>2.322</v>
+        <v>2.302527368205788</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>-6.449999999999999</v>
+        <v>-5.826908916115775</v>
       </c>
       <c r="B184" t="n">
-        <v>2.408</v>
+        <v>2.348933178644198</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>-6.794</v>
+        <v>-6.154263944624652</v>
       </c>
       <c r="B185" t="n">
-        <v>2.408</v>
+        <v>2.36997184953814</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>-6.965999999999999</v>
+        <v>-6.40211289538366</v>
       </c>
       <c r="B186" t="n">
-        <v>2.322</v>
+        <v>2.337290005346325</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>-7.223999999999999</v>
+        <v>-6.660372006804775</v>
       </c>
       <c r="B187" t="n">
-        <v>2.408</v>
+        <v>2.36605567325799</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>-7.481999999999999</v>
+        <v>-6.922755148553383</v>
       </c>
       <c r="B188" t="n">
-        <v>2.322</v>
+        <v>2.336545486537605</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>-7.826</v>
+        <v>-7.228229920602009</v>
       </c>
       <c r="B189" t="n">
-        <v>2.408</v>
+        <v>2.36731938551832</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>-7.997999999999999</v>
+        <v>-7.467441588950736</v>
       </c>
       <c r="B190" t="n">
-        <v>2.58</v>
+        <v>2.467660513590227</v>
       </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>-8.256</v>
+        <v>-7.722193211173808</v>
       </c>
       <c r="B191" t="n">
-        <v>2.408</v>
+        <v>2.426517229849735</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>-8.427999999999999</v>
+        <v>-7.939771908503374</v>
       </c>
       <c r="B192" t="n">
-        <v>2.408</v>
+        <v>2.410210188947197</v>
       </c>
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>-8.686</v>
+        <v>-8.181563397704625</v>
       </c>
       <c r="B193" t="n">
-        <v>2.408</v>
+        <v>2.404153154902371</v>
       </c>
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>-8.857999999999999</v>
+        <v>-8.391601315800965</v>
       </c>
       <c r="B194" t="n">
-        <v>2.408</v>
+        <v>2.403581666618175</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>-9.029999999999999</v>
+        <v>-8.588646225647215</v>
       </c>
       <c r="B195" t="n">
-        <v>2.408</v>
+        <v>2.404257345667228</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>-9.287999999999998</v>
+        <v>-8.82013840660051</v>
       </c>
       <c r="B196" t="n">
-        <v>2.408</v>
+        <v>2.403659916489329</v>
       </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>-9.459999999999999</v>
+        <v>-9.02297478406309</v>
       </c>
       <c r="B197" t="n">
-        <v>2.408</v>
+        <v>2.404566470534883</v>
       </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
-        <v>-9.545999999999999</v>
+        <v>-9.170843587042338</v>
       </c>
       <c r="B198" t="n">
-        <v>2.408</v>
+        <v>2.404138928704382</v>
       </c>
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>-9.803999999999998</v>
+        <v>-9.382732753880124</v>
       </c>
       <c r="B199" t="n">
-        <v>2.408</v>
+        <v>2.405147619288804</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>-9.975999999999999</v>
+        <v>-9.575415776631925</v>
       </c>
       <c r="B200" t="n">
-        <v>2.408</v>
+        <v>2.408834810596599</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>-10.062</v>
+        <v>-9.717480933715365</v>
       </c>
       <c r="B201" t="n">
-        <v>2.322</v>
+        <v>2.365850314735293</v>
       </c>
     </row>
   </sheetData>

</xml_diff>